<commit_message>
Update template excel chung - Format cột ngày là Text
</commit_message>
<xml_diff>
--- a/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
+++ b/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -320,11 +320,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,9 +606,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -617,13 +618,14 @@
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="66.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -648,7 +650,7 @@
       <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -658,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -677,20 +679,21 @@
       <c r="F2">
         <v>23130</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <v>231300</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
       </c>
+      <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -709,20 +712,21 @@
       <c r="F3">
         <v>17340</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>173400</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
       </c>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -741,13 +745,13 @@
       <c r="F4">
         <v>19630</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>392600</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">

</xml_diff>

<commit_message>
chỉnh sửa định dạng cột ngày giao hàng trong template
</commit_message>
<xml_diff>
--- a/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
+++ b/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>EA</t>
   </si>
@@ -42,198 +42,193 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Đơn vị tính
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
+      <t xml:space="preserve">Mã sản phẩm(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tên sản phẩm(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Số lượng 2(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Đơn giá(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thành tiền(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Số PO(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã KH key(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Số lượng 1(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Điền số 1 nếu không có data)</t>
+    </r>
+  </si>
+  <si>
+    <t>85836411-00</t>
+  </si>
+  <si>
+    <t>Trung chuyen C.Quynh-151</t>
+  </si>
+  <si>
+    <t>3101917-7</t>
+  </si>
+  <si>
+    <t>But xoa CP-02</t>
+  </si>
+  <si>
+    <t>3224986-1</t>
+  </si>
+  <si>
+    <t>Hop but sap CR-C05/DO 16mau</t>
+  </si>
+  <si>
+    <t>30/06/2024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày giao hàng
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Không bắt buộc - Định dạng DD/MM/YYYY - Ví dụ: 30/06/2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Đơn vị tính(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>(Không bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã sản phẩm(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên sản phẩm(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng 2(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Đơn giá(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thành tiền(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số PO(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã KH key(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng 1(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Điền số 1 nếu không có data)</t>
-    </r>
-  </si>
-  <si>
-    <t>3101900-3</t>
-  </si>
-  <si>
-    <t>But long mau FP-01-12cay</t>
-  </si>
-  <si>
-    <t>85836411-00</t>
-  </si>
-  <si>
-    <t>Trung chuyen C.Quynh-151</t>
-  </si>
-  <si>
-    <t>3101917-7</t>
-  </si>
-  <si>
-    <t>But xoa CP-02</t>
-  </si>
-  <si>
-    <t>3224986-1</t>
-  </si>
-  <si>
-    <t>Hop but sap CR-C05/DO 16mau</t>
-  </si>
-  <si>
-    <t>30/06/2024</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ngày giao hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Không bắt buộc - Định dạng DD/MM/YYYY - Ví dụ: 30/06/2024)</t>
     </r>
   </si>
 </sst>
@@ -241,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,13 +271,6 @@
     <font>
       <i/>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -309,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -326,6 +314,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,66 +597,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -677,28 +670,28 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>23130</v>
+        <v>17340</v>
       </c>
       <c r="G2" s="4">
-        <v>231300</v>
+        <v>173400</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -707,55 +700,22 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>19630</v>
+      </c>
+      <c r="G3" s="4">
+        <v>392600</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
-        <v>17340</v>
-      </c>
-      <c r="G3" s="4">
-        <v>173400</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>19</v>
+      <c r="I3" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>19630</v>
-      </c>
-      <c r="G4" s="4">
-        <v>392600</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Template excel chung (Khi convert PDF lỗi).xlsx
</commit_message>
<xml_diff>
--- a/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
+++ b/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
@@ -310,13 +310,13 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
@@ -678,7 +678,7 @@
       <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K2" t="s">
@@ -711,7 +711,7 @@
       <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K3" t="s">

</xml_diff>

<commit_message>
Update template excel chung - bỏ bớt cột bắt buộc
</commit_message>
<xml_diff>
--- a/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
+++ b/public/template/excel/Template excel chung (Khi convert PDF lỗi).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
-  <si>
-    <t>EA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <r>
       <t xml:space="preserve">Ghi chú
@@ -42,6 +39,22 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Đơn vị tính
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Không bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Mã sản phẩm(*)
 </t>
     </r>
@@ -59,7 +72,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tên sản phẩm(*)
+      <t xml:space="preserve">Số lượng 2(*)
 </t>
     </r>
     <r>
@@ -76,7 +89,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Số lượng 2(*)
+      <t xml:space="preserve">Số PO(*)
 </t>
     </r>
     <r>
@@ -93,7 +106,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Đơn giá(*)
+      <t xml:space="preserve">Mã KH key(*)
 </t>
     </r>
     <r>
@@ -110,7 +123,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Thành tiền(*)
+      <t xml:space="preserve">Số lượng 1(*)
 </t>
     </r>
     <r>
@@ -122,61 +135,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số PO(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã KH key(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Bắt buộc)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng 1(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>(Điền số 1 nếu không có data)</t>
     </r>
   </si>
   <si>
+    <t>3101900-3</t>
+  </si>
+  <si>
     <t>85836411-00</t>
   </si>
   <si>
@@ -186,19 +151,61 @@
     <t>3101917-7</t>
   </si>
   <si>
-    <t>But xoa CP-02</t>
-  </si>
-  <si>
     <t>3224986-1</t>
   </si>
   <si>
-    <t>Hop but sap CR-C05/DO 16mau</t>
-  </si>
-  <si>
     <t>30/06/2024</t>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Tên sản phẩm
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Không bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Đơn giá
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Không bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thành tiền
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Không bắt buộc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Ngày giao hàng
 </t>
     </r>
@@ -211,24 +218,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Không bắt buộc - Định dạng DD/MM/YYYY - Ví dụ: 30/06/2024)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Đơn vị tính(*)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Không bắt buộc)</t>
+      <t>(Không bắt buộc - Định dạng cột là TEXT, nhập theo DD/MM/YYYY - Ví dụ: 30/06/2024)</t>
     </r>
   </si>
 </sst>
@@ -236,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,7 +261,21 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,13 +314,13 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,71 +601,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="68.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="79.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -669,53 +665,53 @@
       <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>17340</v>
-      </c>
-      <c r="G2" s="4">
-        <v>173400</v>
-      </c>
+      <c r="G2" s="4"/>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>19630</v>
-      </c>
-      <c r="G3" s="4">
-        <v>392600</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
+      <c r="G4" s="4"/>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>